<commit_message>
feat: client google sheet list 구현(#08)
</commit_message>
<xml_diff>
--- a/server/json_to_excel.xlsx
+++ b/server/json_to_excel.xlsx
@@ -397,742 +397,1425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>메뉴코드</v>
+      </c>
+      <c r="B1" t="str">
+        <v>No</v>
+      </c>
+      <c r="C1" t="str">
+        <v>상품코드</v>
+      </c>
+      <c r="D1" t="str">
         <v>상품명</v>
       </c>
-      <c r="B1" t="str">
-        <v>대분류</v>
-      </c>
-      <c r="C1" t="str">
-        <v>거래처</v>
-      </c>
-      <c r="D1" t="str">
-        <v>주문상품구분</v>
+      <c r="E1" t="str">
+        <v>판매가</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>장어 2인</v>
+        <v>0</v>
       </c>
       <c r="B2" t="str">
-        <v>메뉴</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>000001</v>
       </c>
       <c r="D2" t="str">
-        <v>사입상품</v>
+        <v>4 카오팟</v>
+      </c>
+      <c r="E2" t="str">
+        <v>10,000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>장어 1인</v>
+        <v>0</v>
       </c>
       <c r="B3" t="str">
-        <v>메뉴</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
-        <v/>
+        <v>000002</v>
       </c>
       <c r="D3" t="str">
-        <v>사입상품</v>
+        <v>5 카오팟싸파롯</v>
+      </c>
+      <c r="E3" t="str">
+        <v>11,500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>장어 파전골(대)</v>
+        <v>0</v>
       </c>
       <c r="B4" t="str">
-        <v>메뉴</v>
+        <v>3</v>
       </c>
       <c r="C4" t="str">
-        <v/>
+        <v>000003</v>
       </c>
       <c r="D4" t="str">
-        <v>사입상품</v>
+        <v>콜라</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2,000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>장어 파전골(중)</v>
+        <v>0</v>
       </c>
       <c r="B5" t="str">
-        <v>메뉴</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>000004</v>
       </c>
       <c r="D5" t="str">
-        <v>사입상품</v>
+        <v>꿍춧빼텃</v>
+      </c>
+      <c r="E5" t="str">
+        <v>9,500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>파전골 (장어추가)</v>
+        <v>0</v>
       </c>
       <c r="B6" t="str">
-        <v>메뉴</v>
+        <v>5</v>
       </c>
       <c r="C6" t="str">
-        <v/>
+        <v>000005</v>
       </c>
       <c r="D6" t="str">
-        <v>사입상품</v>
+        <v>삑까이텃</v>
+      </c>
+      <c r="E6" t="str">
+        <v>10,000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>정식 (장어)</v>
+        <v>0</v>
       </c>
       <c r="B7" t="str">
-        <v>메뉴</v>
+        <v>6</v>
       </c>
       <c r="C7" t="str">
-        <v/>
+        <v>000006</v>
       </c>
       <c r="D7" t="str">
-        <v>사입상품</v>
+        <v>텃만꿍    2pcs</v>
+      </c>
+      <c r="E7" t="str">
+        <v>6,500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>장어탕</v>
+        <v>0</v>
       </c>
       <c r="B8" t="str">
-        <v>메뉴</v>
+        <v>7</v>
       </c>
       <c r="C8" t="str">
-        <v/>
+        <v>000007</v>
       </c>
       <c r="D8" t="str">
-        <v>사입상품</v>
+        <v>텃만꿍    4pcs</v>
+      </c>
+      <c r="E8" t="str">
+        <v>12,500</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>숯 (추가)</v>
+        <v>0</v>
       </c>
       <c r="B9" t="str">
-        <v>메뉴</v>
+        <v>8</v>
       </c>
       <c r="C9" t="str">
-        <v/>
+        <v>000008</v>
       </c>
       <c r="D9" t="str">
-        <v>사입상품</v>
+        <v>9 팍붕파이댕</v>
+      </c>
+      <c r="E9" t="str">
+        <v>12,500</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>숯 (빼기)</v>
+        <v>0</v>
       </c>
       <c r="B10" t="str">
-        <v>메뉴</v>
+        <v>9</v>
       </c>
       <c r="C10" t="str">
-        <v/>
+        <v>000009</v>
       </c>
       <c r="D10" t="str">
-        <v>사입상품</v>
+        <v>얌운센</v>
+      </c>
+      <c r="E10" t="str">
+        <v>13,000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>초벌용 (숯)</v>
+        <v>0</v>
       </c>
       <c r="B11" t="str">
-        <v>메뉴</v>
+        <v>10</v>
       </c>
       <c r="C11" t="str">
-        <v/>
+        <v>000010</v>
       </c>
       <c r="D11" t="str">
-        <v>사입상품</v>
+        <v>얌살몬</v>
+      </c>
+      <c r="E11" t="str">
+        <v>20,000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2인 포장(완)</v>
+        <v>0</v>
       </c>
       <c r="B12" t="str">
-        <v>포장</v>
+        <v>11</v>
       </c>
       <c r="C12" t="str">
-        <v/>
+        <v>000011</v>
       </c>
       <c r="D12" t="str">
-        <v>사입상품</v>
+        <v>얌탈래</v>
+      </c>
+      <c r="E12" t="str">
+        <v>19,000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>1인 포장(완)</v>
+        <v>0</v>
       </c>
       <c r="B13" t="str">
-        <v>포장</v>
+        <v>12</v>
       </c>
       <c r="C13" t="str">
-        <v/>
+        <v>000012</v>
       </c>
       <c r="D13" t="str">
-        <v>사입상품</v>
+        <v>쏨땀타이</v>
+      </c>
+      <c r="E13" t="str">
+        <v>15,000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2인초벌 (포장)</v>
+        <v>0</v>
       </c>
       <c r="B14" t="str">
-        <v>포장</v>
+        <v>13</v>
       </c>
       <c r="C14" t="str">
-        <v/>
+        <v>000013</v>
       </c>
       <c r="D14" t="str">
-        <v>사입상품</v>
+        <v>쏨땀살몬</v>
+      </c>
+      <c r="E14" t="str">
+        <v>21,000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>생물 (포장)</v>
+        <v>0</v>
       </c>
       <c r="B15" t="str">
-        <v>포장</v>
+        <v>14</v>
       </c>
       <c r="C15" t="str">
-        <v/>
+        <v>000014</v>
       </c>
       <c r="D15" t="str">
-        <v>사입상품</v>
+        <v>6 카오팟싸파롯 순한맛</v>
+      </c>
+      <c r="E15" t="str">
+        <v>11,500</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>장어 엑기스</v>
+        <v>0</v>
       </c>
       <c r="B16" t="str">
-        <v>포장</v>
+        <v>15</v>
       </c>
       <c r="C16" t="str">
-        <v/>
+        <v>000015</v>
       </c>
       <c r="D16" t="str">
-        <v>사입상품</v>
+        <v>7 파카파오 무쌉</v>
+      </c>
+      <c r="E16" t="str">
+        <v>11,000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>파김치(포장)</v>
+        <v>0</v>
       </c>
       <c r="B17" t="str">
-        <v>포장</v>
+        <v>16</v>
       </c>
       <c r="C17" t="str">
-        <v/>
+        <v>000016</v>
       </c>
       <c r="D17" t="str">
-        <v>사입상품</v>
+        <v>8 파카파오 무쌉 순한맛</v>
+      </c>
+      <c r="E17" t="str">
+        <v>11,000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>얼큰라면</v>
+        <v>0</v>
       </c>
       <c r="B18" t="str">
-        <v>사이드</v>
+        <v>17</v>
       </c>
       <c r="C18" t="str">
-        <v/>
+        <v>000017</v>
       </c>
       <c r="D18" t="str">
-        <v>사입상품</v>
+        <v>2 꿍팟퐁커리</v>
+      </c>
+      <c r="E18" t="str">
+        <v>12,000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>된장찌개</v>
+        <v>0</v>
       </c>
       <c r="B19" t="str">
-        <v>사이드</v>
+        <v>18</v>
       </c>
       <c r="C19" t="str">
-        <v/>
+        <v>000018</v>
       </c>
       <c r="D19" t="str">
-        <v>사입상품</v>
+        <v>돔얌꿍 (S) + 밥</v>
+      </c>
+      <c r="E19" t="str">
+        <v>12,500</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>계란찜</v>
+        <v>0</v>
       </c>
       <c r="B20" t="str">
-        <v>사이드</v>
+        <v>19</v>
       </c>
       <c r="C20" t="str">
-        <v/>
+        <v>000019</v>
       </c>
       <c r="D20" t="str">
-        <v>사입상품</v>
+        <v>돔얌꿍 (L)</v>
+      </c>
+      <c r="E20" t="str">
+        <v>20,000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>공기밥</v>
+        <v>0</v>
       </c>
       <c r="B21" t="str">
-        <v>사이드</v>
+        <v>20</v>
       </c>
       <c r="C21" t="str">
-        <v/>
+        <v>000020</v>
       </c>
       <c r="D21" t="str">
-        <v>사입상품</v>
+        <v>1 팟타이</v>
+      </c>
+      <c r="E21" t="str">
+        <v>12,500</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>라면사리</v>
+        <v>0</v>
       </c>
       <c r="B22" t="str">
-        <v>사이드</v>
+        <v>21</v>
       </c>
       <c r="C22" t="str">
-        <v/>
+        <v>000021</v>
       </c>
       <c r="D22" t="str">
-        <v>사입상품</v>
+        <v>꾸에띠어우 까이</v>
+      </c>
+      <c r="E22" t="str">
+        <v>11,500</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>참이슬(후)</v>
+        <v>0</v>
       </c>
       <c r="B23" t="str">
-        <v>주류/음료</v>
+        <v>22</v>
       </c>
       <c r="C23" t="str">
-        <v/>
+        <v>000022</v>
       </c>
       <c r="D23" t="str">
-        <v>사입상품</v>
+        <v>3 뿌팟퐁커리</v>
+      </c>
+      <c r="E23" t="str">
+        <v>26,000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>참이슬(오)</v>
+        <v>0</v>
       </c>
       <c r="B24" t="str">
-        <v>주류/음료</v>
+        <v>23</v>
       </c>
       <c r="C24" t="str">
-        <v/>
+        <v>000023</v>
       </c>
       <c r="D24" t="str">
-        <v>사입상품</v>
+        <v>10 꿍팟멧마무엉</v>
+      </c>
+      <c r="E24" t="str">
+        <v>20,000</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>처음처럼</v>
+        <v>0</v>
       </c>
       <c r="B25" t="str">
-        <v>주류/음료</v>
+        <v>24</v>
       </c>
       <c r="C25" t="str">
-        <v/>
+        <v>000024</v>
       </c>
       <c r="D25" t="str">
-        <v>사입상품</v>
+        <v>밥 추가</v>
+      </c>
+      <c r="E25" t="str">
+        <v>1,000</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>진로이즈백</v>
+        <v>0</v>
       </c>
       <c r="B26" t="str">
-        <v>주류/음료</v>
+        <v>25</v>
       </c>
       <c r="C26" t="str">
-        <v/>
+        <v>000025</v>
       </c>
       <c r="D26" t="str">
-        <v>사입상품</v>
+        <v>운센 hot</v>
+      </c>
+      <c r="E26" t="str">
+        <v>2,000</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>새로</v>
+        <v>0</v>
       </c>
       <c r="B27" t="str">
-        <v>주류/음료</v>
+        <v>26</v>
       </c>
       <c r="C27" t="str">
-        <v/>
+        <v>000026</v>
       </c>
       <c r="D27" t="str">
-        <v>사입상품</v>
+        <v>고수 추가</v>
+      </c>
+      <c r="E27" t="str">
+        <v>1,000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>카스</v>
+        <v>0</v>
       </c>
       <c r="B28" t="str">
-        <v>주류/음료</v>
+        <v>27</v>
       </c>
       <c r="C28" t="str">
-        <v/>
+        <v>000027</v>
       </c>
       <c r="D28" t="str">
-        <v>사입상품</v>
+        <v>라임 추가</v>
+      </c>
+      <c r="E28" t="str">
+        <v>1,000</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>테라</v>
+        <v>0</v>
       </c>
       <c r="B29" t="str">
-        <v>주류/음료</v>
+        <v>28</v>
       </c>
       <c r="C29" t="str">
-        <v/>
+        <v>000028</v>
       </c>
       <c r="D29" t="str">
-        <v>사입상품</v>
+        <v>제로콜라</v>
+      </c>
+      <c r="E29" t="str">
+        <v>2,000</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>보해 복분자</v>
+        <v>0</v>
       </c>
       <c r="B30" t="str">
-        <v>주류/음료</v>
+        <v>29</v>
       </c>
       <c r="C30" t="str">
-        <v/>
+        <v>000029</v>
       </c>
       <c r="D30" t="str">
-        <v>사입상품</v>
+        <v>사이다</v>
+      </c>
+      <c r="E30" t="str">
+        <v>2,000</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>뽕(오디)와인</v>
+        <v>0</v>
       </c>
       <c r="B31" t="str">
-        <v>주류/음료</v>
+        <v>30</v>
       </c>
       <c r="C31" t="str">
-        <v/>
+        <v>000030</v>
       </c>
       <c r="D31" t="str">
-        <v>사입상품</v>
+        <v>제로사이다</v>
+      </c>
+      <c r="E31" t="str">
+        <v>2,000</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>고창 복분자</v>
+        <v>0</v>
       </c>
       <c r="B32" t="str">
-        <v>주류/음료</v>
+        <v>31</v>
       </c>
       <c r="C32" t="str">
-        <v/>
+        <v>000031</v>
       </c>
       <c r="D32" t="str">
-        <v>사입상품</v>
+        <v>아메리카노 Hot</v>
+      </c>
+      <c r="E32" t="str">
+        <v>3,800</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>백세주</v>
+        <v>0</v>
       </c>
       <c r="B33" t="str">
-        <v>주류/음료</v>
+        <v>32</v>
       </c>
       <c r="C33" t="str">
-        <v/>
+        <v>000032</v>
       </c>
       <c r="D33" t="str">
-        <v>사입상품</v>
+        <v>아메리카노 Ice</v>
+      </c>
+      <c r="E33" t="str">
+        <v>3,800</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>청하</v>
+        <v>0</v>
       </c>
       <c r="B34" t="str">
-        <v>주류/음료</v>
+        <v>33</v>
       </c>
       <c r="C34" t="str">
-        <v/>
+        <v>000033</v>
       </c>
       <c r="D34" t="str">
-        <v>사입상품</v>
+        <v>코코넛라떼</v>
+      </c>
+      <c r="E34" t="str">
+        <v>5,000</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>막걸리</v>
+        <v>0</v>
       </c>
       <c r="B35" t="str">
-        <v>주류/음료</v>
+        <v>34</v>
       </c>
       <c r="C35" t="str">
-        <v/>
+        <v>000034</v>
       </c>
       <c r="D35" t="str">
-        <v>사입상품</v>
+        <v>커피반치앙마이</v>
+      </c>
+      <c r="E35" t="str">
+        <v>5,500</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>코카콜라</v>
+        <v>0</v>
       </c>
       <c r="B36" t="str">
-        <v>주류/음료</v>
+        <v>35</v>
       </c>
       <c r="C36" t="str">
-        <v/>
+        <v>000035</v>
       </c>
       <c r="D36" t="str">
-        <v>사입상품</v>
+        <v>카페보란</v>
+      </c>
+      <c r="E36" t="str">
+        <v>5,000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>사이다</v>
+        <v>0</v>
       </c>
       <c r="B37" t="str">
-        <v>주류/음료</v>
+        <v>36</v>
       </c>
       <c r="C37" t="str">
-        <v/>
+        <v>000036</v>
       </c>
       <c r="D37" t="str">
-        <v>사입상품</v>
+        <v>차놈옌</v>
+      </c>
+      <c r="E37" t="str">
+        <v>4,500</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>환타</v>
+        <v>0</v>
       </c>
       <c r="B38" t="str">
-        <v>주류/음료</v>
+        <v>37</v>
       </c>
       <c r="C38" t="str">
-        <v/>
+        <v>000037</v>
       </c>
       <c r="D38" t="str">
-        <v>사입상품</v>
+        <v>코코넛워터</v>
+      </c>
+      <c r="E38" t="str">
+        <v>4,500</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>*계란찜 (서비스)</v>
+        <v>0</v>
       </c>
       <c r="B39" t="str">
-        <v>서비스</v>
+        <v>38</v>
       </c>
       <c r="C39" t="str">
-        <v/>
+        <v>000038</v>
       </c>
       <c r="D39" t="str">
-        <v>사입상품</v>
+        <v>망고스틴리치</v>
+      </c>
+      <c r="E39" t="str">
+        <v>4,000</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>*장어탕 (서비스)</v>
+        <v>0</v>
       </c>
       <c r="B40" t="str">
-        <v>서비스</v>
+        <v>39</v>
       </c>
       <c r="C40" t="str">
-        <v/>
+        <v>000039</v>
       </c>
       <c r="D40" t="str">
-        <v>사입상품</v>
+        <v>망고스틴파인</v>
+      </c>
+      <c r="E40" t="str">
+        <v>4,000</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>*된장찌개 (서비스)</v>
+        <v>0</v>
       </c>
       <c r="B41" t="str">
-        <v>서비스</v>
+        <v>40</v>
       </c>
       <c r="C41" t="str">
-        <v/>
+        <v>000040</v>
       </c>
       <c r="D41" t="str">
-        <v>사입상품</v>
+        <v>패션후르츠 에이드</v>
+      </c>
+      <c r="E41" t="str">
+        <v>5,500</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>수재비 사리</v>
+        <v>0</v>
       </c>
       <c r="B42" t="str">
-        <v>사이드</v>
+        <v>41</v>
       </c>
       <c r="C42" t="str">
-        <v/>
+        <v>000041</v>
       </c>
       <c r="D42" t="str">
-        <v>사입상품</v>
+        <v>리치 에이드</v>
+      </c>
+      <c r="E42" t="str">
+        <v>5,500</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>장어탕 (포장)</v>
+        <v>0</v>
       </c>
       <c r="B43" t="str">
-        <v>포장</v>
+        <v>42</v>
       </c>
       <c r="C43" t="str">
-        <v/>
+        <v>000042</v>
       </c>
       <c r="D43" t="str">
-        <v>사입상품</v>
+        <v>오로라옌옌</v>
+      </c>
+      <c r="E43" t="str">
+        <v>6,000</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>(포장) 장어파전골(중)</v>
+        <v>0</v>
       </c>
       <c r="B44" t="str">
-        <v>포장</v>
+        <v>43</v>
       </c>
       <c r="C44" t="str">
-        <v/>
+        <v>000043</v>
       </c>
       <c r="D44" t="str">
-        <v>사입상품</v>
+        <v>테라생맥주</v>
+      </c>
+      <c r="E44" t="str">
+        <v>5,000</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>(포장) 장어파전골(대)</v>
+        <v>0</v>
       </c>
       <c r="B45" t="str">
-        <v>포장</v>
+        <v>44</v>
       </c>
       <c r="C45" t="str">
-        <v/>
+        <v>000044</v>
       </c>
       <c r="D45" t="str">
-        <v>사입상품</v>
+        <v>블랑생맥주</v>
+      </c>
+      <c r="E45" t="str">
+        <v>7,000</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>씨앗강정</v>
+        <v>0</v>
       </c>
       <c r="B46" t="str">
-        <v>과자</v>
+        <v>45</v>
       </c>
       <c r="C46" t="str">
-        <v/>
+        <v>000045</v>
       </c>
       <c r="D46" t="str">
-        <v>사입상품</v>
+        <v>처음처럼</v>
+      </c>
+      <c r="E46" t="str">
+        <v>5,000</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>검은깨강정</v>
+        <v>0</v>
       </c>
       <c r="B47" t="str">
-        <v>과자</v>
+        <v>46</v>
       </c>
       <c r="C47" t="str">
-        <v/>
+        <v>000046</v>
       </c>
       <c r="D47" t="str">
-        <v>사입상품</v>
+        <v>참이슬</v>
+      </c>
+      <c r="E47" t="str">
+        <v>5,000</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>메밀강정</v>
+        <v>0</v>
       </c>
       <c r="B48" t="str">
-        <v>과자</v>
+        <v>47</v>
       </c>
       <c r="C48" t="str">
-        <v/>
+        <v>000047</v>
       </c>
       <c r="D48" t="str">
-        <v>사입상품</v>
+        <v>이즈백</v>
+      </c>
+      <c r="E48" t="str">
+        <v>5,000</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>감귤젤리</v>
+        <v>0</v>
       </c>
       <c r="B49" t="str">
-        <v>과자</v>
+        <v>48</v>
       </c>
       <c r="C49" t="str">
-        <v/>
+        <v>000048</v>
       </c>
       <c r="D49" t="str">
-        <v>사입상품</v>
+        <v>창</v>
+      </c>
+      <c r="E49" t="str">
+        <v>6,000</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>약과</v>
+        <v>0</v>
       </c>
       <c r="B50" t="str">
-        <v>과자</v>
+        <v>49</v>
       </c>
       <c r="C50" t="str">
-        <v/>
+        <v>000049</v>
       </c>
       <c r="D50" t="str">
-        <v>사입상품</v>
+        <v>리오</v>
+      </c>
+      <c r="E50" t="str">
+        <v>6,000</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>잣엿</v>
+        <v>0</v>
       </c>
       <c r="B51" t="str">
-        <v>과자</v>
+        <v>50</v>
       </c>
       <c r="C51" t="str">
-        <v/>
+        <v>000050</v>
       </c>
       <c r="D51" t="str">
-        <v>사입상품</v>
+        <v>하이볼</v>
+      </c>
+      <c r="E51" t="str">
+        <v>6,500</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>정식 (포장)</v>
+        <v>0</v>
       </c>
       <c r="B52" t="str">
-        <v>포장</v>
+        <v>51</v>
       </c>
       <c r="C52" t="str">
-        <v/>
+        <v>000051</v>
       </c>
       <c r="D52" t="str">
-        <v>사입상품</v>
+        <v>쌀국수면</v>
+      </c>
+      <c r="E52" t="str">
+        <v>2,500</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>0</v>
+      </c>
+      <c r="B53" t="str">
+        <v>52</v>
+      </c>
+      <c r="C53" t="str">
+        <v>000052</v>
+      </c>
+      <c r="D53" t="str">
+        <v>take-out</v>
+      </c>
+      <c r="E53" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>0</v>
+      </c>
+      <c r="B54" t="str">
+        <v>53</v>
+      </c>
+      <c r="C54" t="str">
+        <v>000053</v>
+      </c>
+      <c r="D54" t="str">
+        <v>운센 ice</v>
+      </c>
+      <c r="E54" t="str">
+        <v>2,000</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0</v>
+      </c>
+      <c r="B55" t="str">
+        <v>54</v>
+      </c>
+      <c r="C55" t="str">
+        <v>000054</v>
+      </c>
+      <c r="D55" t="str">
+        <v>탄산수</v>
+      </c>
+      <c r="E55" t="str">
+        <v>3,000</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>0</v>
+      </c>
+      <c r="B56" t="str">
+        <v>55</v>
+      </c>
+      <c r="C56" t="str">
+        <v>000055</v>
+      </c>
+      <c r="D56" t="str">
+        <v>서비스 꿍춧빼텃</v>
+      </c>
+      <c r="E56" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>0</v>
+      </c>
+      <c r="B57" t="str">
+        <v>56</v>
+      </c>
+      <c r="C57" t="str">
+        <v>000056</v>
+      </c>
+      <c r="D57" t="str">
+        <v>서비스 삑까이텃</v>
+      </c>
+      <c r="E57" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>0</v>
+      </c>
+      <c r="B58" t="str">
+        <v>57</v>
+      </c>
+      <c r="C58" t="str">
+        <v>000057</v>
+      </c>
+      <c r="D58" t="str">
+        <v>서비스 텃만꿍 2pcs</v>
+      </c>
+      <c r="E58" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>0</v>
+      </c>
+      <c r="B59" t="str">
+        <v>58</v>
+      </c>
+      <c r="C59" t="str">
+        <v>000058</v>
+      </c>
+      <c r="D59" t="str">
+        <v>서비스 얌운센</v>
+      </c>
+      <c r="E59" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>0</v>
+      </c>
+      <c r="B60" t="str">
+        <v>59</v>
+      </c>
+      <c r="C60" t="str">
+        <v>000059</v>
+      </c>
+      <c r="D60" t="str">
+        <v>서비스 카오팟</v>
+      </c>
+      <c r="E60" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>0</v>
+      </c>
+      <c r="B61" t="str">
+        <v>60</v>
+      </c>
+      <c r="C61" t="str">
+        <v>000060</v>
+      </c>
+      <c r="D61" t="str">
+        <v>서비스 파카파오무쌉</v>
+      </c>
+      <c r="E61" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>0</v>
+      </c>
+      <c r="B62" t="str">
+        <v>61</v>
+      </c>
+      <c r="C62" t="str">
+        <v>000061</v>
+      </c>
+      <c r="D62" t="str">
+        <v>서비스 꿍팟퐁커리</v>
+      </c>
+      <c r="E62" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>0</v>
+      </c>
+      <c r="B63" t="str">
+        <v>62</v>
+      </c>
+      <c r="C63" t="str">
+        <v>000062</v>
+      </c>
+      <c r="D63" t="str">
+        <v>서비스 팟타이</v>
+      </c>
+      <c r="E63" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>0</v>
+      </c>
+      <c r="B64" t="str">
+        <v>63</v>
+      </c>
+      <c r="C64" t="str">
+        <v>000063</v>
+      </c>
+      <c r="D64" t="str">
+        <v>서비스 꾸에띠어우</v>
+      </c>
+      <c r="E64" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>0</v>
+      </c>
+      <c r="B65" t="str">
+        <v>64</v>
+      </c>
+      <c r="C65" t="str">
+        <v>000064</v>
+      </c>
+      <c r="D65" t="str">
+        <v>서비스 밥</v>
+      </c>
+      <c r="E65" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>0</v>
+      </c>
+      <c r="B66" t="str">
+        <v>65</v>
+      </c>
+      <c r="C66" t="str">
+        <v>000065</v>
+      </c>
+      <c r="D66" t="str">
+        <v>서비스 당면</v>
+      </c>
+      <c r="E66" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>0</v>
+      </c>
+      <c r="B67" t="str">
+        <v>66</v>
+      </c>
+      <c r="C67" t="str">
+        <v>000066</v>
+      </c>
+      <c r="D67" t="str">
+        <v>서비스 콜라</v>
+      </c>
+      <c r="E67" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>0</v>
+      </c>
+      <c r="B68" t="str">
+        <v>67</v>
+      </c>
+      <c r="C68" t="str">
+        <v>000067</v>
+      </c>
+      <c r="D68" t="str">
+        <v>서비스 사이다</v>
+      </c>
+      <c r="E68" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>0</v>
+      </c>
+      <c r="B69" t="str">
+        <v>68</v>
+      </c>
+      <c r="C69" t="str">
+        <v>000068</v>
+      </c>
+      <c r="D69" t="str">
+        <v>서비스 차놈옌</v>
+      </c>
+      <c r="E69" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>0</v>
+      </c>
+      <c r="B70" t="str">
+        <v>69</v>
+      </c>
+      <c r="C70" t="str">
+        <v>000069</v>
+      </c>
+      <c r="D70" t="str">
+        <v>서비스 망고스틴쥬스</v>
+      </c>
+      <c r="E70" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>0</v>
+      </c>
+      <c r="B71" t="str">
+        <v>70</v>
+      </c>
+      <c r="C71" t="str">
+        <v>000070</v>
+      </c>
+      <c r="D71" t="str">
+        <v>서비스 패션후르츠</v>
+      </c>
+      <c r="E71" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>0</v>
+      </c>
+      <c r="B72" t="str">
+        <v>71</v>
+      </c>
+      <c r="C72" t="str">
+        <v>000071</v>
+      </c>
+      <c r="D72" t="str">
+        <v>서비스 옌옌에이드</v>
+      </c>
+      <c r="E72" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>0</v>
+      </c>
+      <c r="B73" t="str">
+        <v>72</v>
+      </c>
+      <c r="C73" t="str">
+        <v>000072</v>
+      </c>
+      <c r="D73" t="str">
+        <v>서비스 테라생맥주</v>
+      </c>
+      <c r="E73" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>0</v>
+      </c>
+      <c r="B74" t="str">
+        <v>73</v>
+      </c>
+      <c r="C74" t="str">
+        <v>000073</v>
+      </c>
+      <c r="D74" t="str">
+        <v>서비스 소주</v>
+      </c>
+      <c r="E74" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>0</v>
+      </c>
+      <c r="B75" t="str">
+        <v>74</v>
+      </c>
+      <c r="C75" t="str">
+        <v>000074</v>
+      </c>
+      <c r="D75" t="str">
+        <v>l__ 맵게(very spicy)</v>
+      </c>
+      <c r="E75" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>0</v>
+      </c>
+      <c r="B76" t="str">
+        <v>75</v>
+      </c>
+      <c r="C76" t="str">
+        <v>000075</v>
+      </c>
+      <c r="D76" t="str">
+        <v>l__ 덜 맵게(less spicy)</v>
+      </c>
+      <c r="E76" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>0</v>
+      </c>
+      <c r="B77" t="str">
+        <v>76</v>
+      </c>
+      <c r="C77" t="str">
+        <v>000076</v>
+      </c>
+      <c r="D77" t="str">
+        <v>l__ 안 맵게(no spicy)</v>
+      </c>
+      <c r="E77" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>0</v>
+      </c>
+      <c r="B78" t="str">
+        <v>77</v>
+      </c>
+      <c r="C78" t="str">
+        <v>000077</v>
+      </c>
+      <c r="D78" t="str">
+        <v>l__ 싱겁게(less solty)</v>
+      </c>
+      <c r="E78" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>0</v>
+      </c>
+      <c r="B79" t="str">
+        <v>78</v>
+      </c>
+      <c r="C79" t="str">
+        <v>000078</v>
+      </c>
+      <c r="D79" t="str">
+        <v>수끼남</v>
+      </c>
+      <c r="E79" t="str">
+        <v>11,500</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>0</v>
+      </c>
+      <c r="B80" t="str">
+        <v>79</v>
+      </c>
+      <c r="C80" t="str">
+        <v>000079</v>
+      </c>
+      <c r="D80" t="str">
+        <v>11 텃2+팟+꿍+쏨</v>
+      </c>
+      <c r="E80" t="str">
+        <v>45,000</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>0</v>
+      </c>
+      <c r="B81" t="str">
+        <v>80</v>
+      </c>
+      <c r="C81" t="str">
+        <v>000080</v>
+      </c>
+      <c r="D81" t="str">
+        <v>포장용기</v>
+      </c>
+      <c r="E81" t="str">
+        <v>1,000</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>0</v>
+      </c>
+      <c r="B82" t="str">
+        <v>81</v>
+      </c>
+      <c r="C82" t="str">
+        <v>000081</v>
+      </c>
+      <c r="D82" t="str">
+        <v>호가든 무알콜</v>
+      </c>
+      <c r="E82" t="str">
+        <v>6,000</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>0</v>
+      </c>
+      <c r="B83" t="str">
+        <v>82</v>
+      </c>
+      <c r="C83" t="str">
+        <v>000082</v>
+      </c>
+      <c r="D83" t="str">
+        <v>새로</v>
+      </c>
+      <c r="E83" t="str">
+        <v>5,000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D52"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E83"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>